<commit_message>
Update reference file: Y4_B2526_General_&_Special_Surgery_1_B1_reference_data.xlsx
</commit_message>
<xml_diff>
--- a/reference_data/Y4_B2526_General_&_Special_Surgery_1_B1_reference_data.xlsx
+++ b/reference_data/Y4_B2526_General_&_Special_Surgery_1_B1_reference_data.xlsx
@@ -454,7 +454,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E320"/>
+  <dimension ref="A1:E321"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,7 +519,7 @@
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -546,7 +546,7 @@
       </c>
       <c r="E3" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -573,7 +573,7 @@
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -600,7 +600,7 @@
       </c>
       <c r="E5" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -627,7 +627,7 @@
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -654,7 +654,7 @@
       </c>
       <c r="E7" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -681,7 +681,7 @@
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -708,7 +708,7 @@
       </c>
       <c r="E9" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -735,7 +735,7 @@
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -762,7 +762,7 @@
       </c>
       <c r="E11" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -789,7 +789,7 @@
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -816,7 +816,7 @@
       </c>
       <c r="E13" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -843,7 +843,7 @@
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -870,7 +870,7 @@
       </c>
       <c r="E15" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -897,7 +897,7 @@
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -924,7 +924,7 @@
       </c>
       <c r="E17" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -951,7 +951,7 @@
       </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -978,7 +978,7 @@
       </c>
       <c r="E19" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1005,7 +1005,7 @@
       </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1032,7 +1032,7 @@
       </c>
       <c r="E21" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="E22" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1086,7 +1086,7 @@
       </c>
       <c r="E23" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1113,7 +1113,7 @@
       </c>
       <c r="E24" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1140,7 +1140,7 @@
       </c>
       <c r="E25" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1167,7 +1167,7 @@
       </c>
       <c r="E26" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1194,7 +1194,7 @@
       </c>
       <c r="E27" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1221,7 +1221,7 @@
       </c>
       <c r="E28" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1248,7 +1248,7 @@
       </c>
       <c r="E29" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1275,7 +1275,7 @@
       </c>
       <c r="E30" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1302,7 +1302,7 @@
       </c>
       <c r="E31" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1329,7 +1329,7 @@
       </c>
       <c r="E32" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1356,7 +1356,7 @@
       </c>
       <c r="E33" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1383,7 +1383,7 @@
       </c>
       <c r="E34" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1410,7 +1410,7 @@
       </c>
       <c r="E35" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1437,7 +1437,7 @@
       </c>
       <c r="E36" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1464,7 +1464,7 @@
       </c>
       <c r="E37" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1491,7 +1491,7 @@
       </c>
       <c r="E38" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1518,7 +1518,7 @@
       </c>
       <c r="E39" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="E40" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1572,7 +1572,7 @@
       </c>
       <c r="E41" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1599,7 +1599,7 @@
       </c>
       <c r="E42" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1626,7 +1626,7 @@
       </c>
       <c r="E43" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1653,7 +1653,7 @@
       </c>
       <c r="E44" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1680,7 +1680,7 @@
       </c>
       <c r="E45" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1707,7 +1707,7 @@
       </c>
       <c r="E46" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1734,7 +1734,7 @@
       </c>
       <c r="E47" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1761,7 +1761,7 @@
       </c>
       <c r="E48" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1788,7 +1788,7 @@
       </c>
       <c r="E49" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1815,7 +1815,7 @@
       </c>
       <c r="E50" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1842,7 +1842,7 @@
       </c>
       <c r="E51" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1869,7 +1869,7 @@
       </c>
       <c r="E52" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1896,7 +1896,7 @@
       </c>
       <c r="E53" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1923,7 +1923,7 @@
       </c>
       <c r="E54" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1950,7 +1950,7 @@
       </c>
       <c r="E55" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -1977,7 +1977,7 @@
       </c>
       <c r="E56" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2004,7 +2004,7 @@
       </c>
       <c r="E57" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2031,7 +2031,7 @@
       </c>
       <c r="E58" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2058,7 +2058,7 @@
       </c>
       <c r="E59" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2085,7 +2085,7 @@
       </c>
       <c r="E60" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2112,7 +2112,7 @@
       </c>
       <c r="E61" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2139,7 +2139,7 @@
       </c>
       <c r="E62" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2166,7 +2166,7 @@
       </c>
       <c r="E63" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2193,7 +2193,7 @@
       </c>
       <c r="E64" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2220,7 +2220,7 @@
       </c>
       <c r="E65" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2247,7 +2247,7 @@
       </c>
       <c r="E66" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2274,7 +2274,7 @@
       </c>
       <c r="E67" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2301,7 +2301,7 @@
       </c>
       <c r="E68" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2328,7 +2328,7 @@
       </c>
       <c r="E69" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2355,7 +2355,7 @@
       </c>
       <c r="E70" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2382,7 +2382,7 @@
       </c>
       <c r="E71" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2409,7 +2409,7 @@
       </c>
       <c r="E72" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2436,7 +2436,7 @@
       </c>
       <c r="E73" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2463,7 +2463,7 @@
       </c>
       <c r="E74" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2490,7 +2490,7 @@
       </c>
       <c r="E75" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2517,7 +2517,7 @@
       </c>
       <c r="E76" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2544,7 +2544,7 @@
       </c>
       <c r="E77" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2571,7 +2571,7 @@
       </c>
       <c r="E78" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2598,7 +2598,7 @@
       </c>
       <c r="E79" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2625,7 +2625,7 @@
       </c>
       <c r="E80" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2652,7 +2652,7 @@
       </c>
       <c r="E81" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2679,7 +2679,7 @@
       </c>
       <c r="E82" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2706,7 +2706,7 @@
       </c>
       <c r="E83" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2733,7 +2733,7 @@
       </c>
       <c r="E84" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2760,7 +2760,7 @@
       </c>
       <c r="E85" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2787,7 +2787,7 @@
       </c>
       <c r="E86" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2814,7 +2814,7 @@
       </c>
       <c r="E87" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2841,7 +2841,7 @@
       </c>
       <c r="E88" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2868,7 +2868,7 @@
       </c>
       <c r="E89" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2895,7 +2895,7 @@
       </c>
       <c r="E90" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2922,7 +2922,7 @@
       </c>
       <c r="E91" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2949,7 +2949,7 @@
       </c>
       <c r="E92" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -2976,7 +2976,7 @@
       </c>
       <c r="E93" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3003,7 +3003,7 @@
       </c>
       <c r="E94" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3030,7 +3030,7 @@
       </c>
       <c r="E95" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3057,7 +3057,7 @@
       </c>
       <c r="E96" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3084,7 +3084,7 @@
       </c>
       <c r="E97" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3111,7 +3111,7 @@
       </c>
       <c r="E98" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3138,7 +3138,7 @@
       </c>
       <c r="E99" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3165,7 +3165,7 @@
       </c>
       <c r="E100" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3192,7 +3192,7 @@
       </c>
       <c r="E101" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3219,7 +3219,7 @@
       </c>
       <c r="E102" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3246,7 +3246,7 @@
       </c>
       <c r="E103" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3273,7 +3273,7 @@
       </c>
       <c r="E104" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3300,7 +3300,7 @@
       </c>
       <c r="E105" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3327,7 +3327,7 @@
       </c>
       <c r="E106" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3354,7 +3354,7 @@
       </c>
       <c r="E107" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3381,7 +3381,7 @@
       </c>
       <c r="E108" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3408,7 +3408,7 @@
       </c>
       <c r="E109" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3435,7 +3435,7 @@
       </c>
       <c r="E110" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3462,7 +3462,7 @@
       </c>
       <c r="E111" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3489,7 +3489,7 @@
       </c>
       <c r="E112" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3516,7 +3516,7 @@
       </c>
       <c r="E113" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3543,7 +3543,7 @@
       </c>
       <c r="E114" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3570,7 +3570,7 @@
       </c>
       <c r="E115" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3597,7 +3597,7 @@
       </c>
       <c r="E116" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3624,7 +3624,7 @@
       </c>
       <c r="E117" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3651,7 +3651,7 @@
       </c>
       <c r="E118" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3678,7 +3678,7 @@
       </c>
       <c r="E119" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3705,7 +3705,7 @@
       </c>
       <c r="E120" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3732,7 +3732,7 @@
       </c>
       <c r="E121" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3759,7 +3759,7 @@
       </c>
       <c r="E122" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3786,7 +3786,7 @@
       </c>
       <c r="E123" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3813,7 +3813,7 @@
       </c>
       <c r="E124" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3840,7 +3840,7 @@
       </c>
       <c r="E125" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3867,7 +3867,7 @@
       </c>
       <c r="E126" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3894,7 +3894,7 @@
       </c>
       <c r="E127" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3921,7 +3921,7 @@
       </c>
       <c r="E128" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3948,7 +3948,7 @@
       </c>
       <c r="E129" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -3975,7 +3975,7 @@
       </c>
       <c r="E130" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4002,7 +4002,7 @@
       </c>
       <c r="E131" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4029,7 +4029,7 @@
       </c>
       <c r="E132" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4056,7 +4056,7 @@
       </c>
       <c r="E133" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4083,7 +4083,7 @@
       </c>
       <c r="E134" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4110,7 +4110,7 @@
       </c>
       <c r="E135" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4137,7 +4137,7 @@
       </c>
       <c r="E136" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4164,7 +4164,7 @@
       </c>
       <c r="E137" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4191,7 +4191,7 @@
       </c>
       <c r="E138" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4218,7 +4218,7 @@
       </c>
       <c r="E139" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4245,7 +4245,7 @@
       </c>
       <c r="E140" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4272,7 +4272,7 @@
       </c>
       <c r="E141" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4299,7 +4299,7 @@
       </c>
       <c r="E142" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4326,7 +4326,7 @@
       </c>
       <c r="E143" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4353,7 +4353,7 @@
       </c>
       <c r="E144" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4380,7 +4380,7 @@
       </c>
       <c r="E145" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4407,7 +4407,7 @@
       </c>
       <c r="E146" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4434,7 +4434,7 @@
       </c>
       <c r="E147" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4461,7 +4461,7 @@
       </c>
       <c r="E148" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4488,7 +4488,7 @@
       </c>
       <c r="E149" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4515,7 +4515,7 @@
       </c>
       <c r="E150" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4542,7 +4542,7 @@
       </c>
       <c r="E151" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4569,7 +4569,7 @@
       </c>
       <c r="E152" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4596,7 +4596,7 @@
       </c>
       <c r="E153" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4623,7 +4623,7 @@
       </c>
       <c r="E154" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4650,7 +4650,7 @@
       </c>
       <c r="E155" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4677,7 +4677,7 @@
       </c>
       <c r="E156" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4704,7 +4704,7 @@
       </c>
       <c r="E157" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4731,7 +4731,7 @@
       </c>
       <c r="E158" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4758,7 +4758,7 @@
       </c>
       <c r="E159" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4785,7 +4785,7 @@
       </c>
       <c r="E160" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4812,7 +4812,7 @@
       </c>
       <c r="E161" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4839,7 +4839,7 @@
       </c>
       <c r="E162" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4866,7 +4866,7 @@
       </c>
       <c r="E163" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4893,7 +4893,7 @@
       </c>
       <c r="E164" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4920,7 +4920,7 @@
       </c>
       <c r="E165" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4947,7 +4947,7 @@
       </c>
       <c r="E166" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -4974,7 +4974,7 @@
       </c>
       <c r="E167" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5001,7 +5001,7 @@
       </c>
       <c r="E168" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5028,7 +5028,7 @@
       </c>
       <c r="E169" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5055,7 +5055,7 @@
       </c>
       <c r="E170" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5082,7 +5082,7 @@
       </c>
       <c r="E171" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5109,7 +5109,7 @@
       </c>
       <c r="E172" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5136,7 +5136,7 @@
       </c>
       <c r="E173" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5163,7 +5163,7 @@
       </c>
       <c r="E174" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5190,7 +5190,7 @@
       </c>
       <c r="E175" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5217,7 +5217,7 @@
       </c>
       <c r="E176" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5244,7 +5244,7 @@
       </c>
       <c r="E177" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5271,7 +5271,7 @@
       </c>
       <c r="E178" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5298,7 +5298,7 @@
       </c>
       <c r="E179" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5325,7 +5325,7 @@
       </c>
       <c r="E180" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5352,7 +5352,7 @@
       </c>
       <c r="E181" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5379,7 +5379,7 @@
       </c>
       <c r="E182" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5406,7 +5406,7 @@
       </c>
       <c r="E183" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5433,7 +5433,7 @@
       </c>
       <c r="E184" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5460,7 +5460,7 @@
       </c>
       <c r="E185" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5487,7 +5487,7 @@
       </c>
       <c r="E186" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5514,7 +5514,7 @@
       </c>
       <c r="E187" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5541,7 +5541,7 @@
       </c>
       <c r="E188" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5568,7 +5568,7 @@
       </c>
       <c r="E189" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5595,7 +5595,7 @@
       </c>
       <c r="E190" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5622,7 +5622,7 @@
       </c>
       <c r="E191" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5649,7 +5649,7 @@
       </c>
       <c r="E192" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5676,7 +5676,7 @@
       </c>
       <c r="E193" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5703,7 +5703,7 @@
       </c>
       <c r="E194" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5730,7 +5730,7 @@
       </c>
       <c r="E195" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5757,7 +5757,7 @@
       </c>
       <c r="E196" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5784,7 +5784,7 @@
       </c>
       <c r="E197" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5811,7 +5811,7 @@
       </c>
       <c r="E198" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5838,7 +5838,7 @@
       </c>
       <c r="E199" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5865,7 +5865,7 @@
       </c>
       <c r="E200" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5892,7 +5892,7 @@
       </c>
       <c r="E201" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5919,7 +5919,7 @@
       </c>
       <c r="E202" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5946,7 +5946,7 @@
       </c>
       <c r="E203" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -5973,7 +5973,7 @@
       </c>
       <c r="E204" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6000,7 +6000,7 @@
       </c>
       <c r="E205" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6027,7 +6027,7 @@
       </c>
       <c r="E206" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6054,7 +6054,7 @@
       </c>
       <c r="E207" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6081,7 +6081,7 @@
       </c>
       <c r="E208" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6108,7 +6108,7 @@
       </c>
       <c r="E209" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6135,7 +6135,7 @@
       </c>
       <c r="E210" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6162,7 +6162,7 @@
       </c>
       <c r="E211" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6189,7 +6189,7 @@
       </c>
       <c r="E212" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6216,7 +6216,7 @@
       </c>
       <c r="E213" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6243,7 +6243,7 @@
       </c>
       <c r="E214" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6270,7 +6270,7 @@
       </c>
       <c r="E215" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6297,7 +6297,7 @@
       </c>
       <c r="E216" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6324,7 +6324,7 @@
       </c>
       <c r="E217" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6351,7 +6351,7 @@
       </c>
       <c r="E218" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6378,7 +6378,7 @@
       </c>
       <c r="E219" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6405,7 +6405,7 @@
       </c>
       <c r="E220" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6432,7 +6432,7 @@
       </c>
       <c r="E221" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6459,7 +6459,7 @@
       </c>
       <c r="E222" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6486,7 +6486,7 @@
       </c>
       <c r="E223" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6513,7 +6513,7 @@
       </c>
       <c r="E224" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6540,7 +6540,7 @@
       </c>
       <c r="E225" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6567,7 +6567,7 @@
       </c>
       <c r="E226" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6594,7 +6594,7 @@
       </c>
       <c r="E227" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6621,7 +6621,7 @@
       </c>
       <c r="E228" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6648,7 +6648,7 @@
       </c>
       <c r="E229" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6675,7 +6675,7 @@
       </c>
       <c r="E230" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6702,7 +6702,7 @@
       </c>
       <c r="E231" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6729,7 +6729,7 @@
       </c>
       <c r="E232" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6756,7 +6756,7 @@
       </c>
       <c r="E233" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6783,7 +6783,7 @@
       </c>
       <c r="E234" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6810,7 +6810,7 @@
       </c>
       <c r="E235" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6837,7 +6837,7 @@
       </c>
       <c r="E236" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6864,7 +6864,7 @@
       </c>
       <c r="E237" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6891,7 +6891,7 @@
       </c>
       <c r="E238" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6918,7 +6918,7 @@
       </c>
       <c r="E239" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6945,7 +6945,7 @@
       </c>
       <c r="E240" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6972,7 +6972,7 @@
       </c>
       <c r="E241" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -6999,7 +6999,7 @@
       </c>
       <c r="E242" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7026,7 +7026,7 @@
       </c>
       <c r="E243" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7053,7 +7053,7 @@
       </c>
       <c r="E244" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7080,7 +7080,7 @@
       </c>
       <c r="E245" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7107,7 +7107,7 @@
       </c>
       <c r="E246" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7134,7 +7134,7 @@
       </c>
       <c r="E247" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7161,7 +7161,7 @@
       </c>
       <c r="E248" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7188,7 +7188,7 @@
       </c>
       <c r="E249" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7215,7 +7215,7 @@
       </c>
       <c r="E250" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7242,7 +7242,7 @@
       </c>
       <c r="E251" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7269,7 +7269,7 @@
       </c>
       <c r="E252" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7296,7 +7296,7 @@
       </c>
       <c r="E253" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7323,7 +7323,7 @@
       </c>
       <c r="E254" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7350,7 +7350,7 @@
       </c>
       <c r="E255" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7377,7 +7377,7 @@
       </c>
       <c r="E256" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7404,7 +7404,7 @@
       </c>
       <c r="E257" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7431,7 +7431,7 @@
       </c>
       <c r="E258" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7458,7 +7458,7 @@
       </c>
       <c r="E259" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7485,7 +7485,7 @@
       </c>
       <c r="E260" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7512,7 +7512,7 @@
       </c>
       <c r="E261" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7539,7 +7539,7 @@
       </c>
       <c r="E262" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7566,7 +7566,7 @@
       </c>
       <c r="E263" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7593,7 +7593,7 @@
       </c>
       <c r="E264" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7620,7 +7620,7 @@
       </c>
       <c r="E265" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7647,7 +7647,7 @@
       </c>
       <c r="E266" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7674,7 +7674,7 @@
       </c>
       <c r="E267" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7701,7 +7701,7 @@
       </c>
       <c r="E268" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7728,7 +7728,7 @@
       </c>
       <c r="E269" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7755,7 +7755,7 @@
       </c>
       <c r="E270" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7782,7 +7782,7 @@
       </c>
       <c r="E271" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7809,7 +7809,7 @@
       </c>
       <c r="E272" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7836,7 +7836,7 @@
       </c>
       <c r="E273" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7863,7 +7863,7 @@
       </c>
       <c r="E274" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7890,7 +7890,7 @@
       </c>
       <c r="E275" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7917,7 +7917,7 @@
       </c>
       <c r="E276" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7944,7 +7944,7 @@
       </c>
       <c r="E277" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7971,7 +7971,7 @@
       </c>
       <c r="E278" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -7998,7 +7998,7 @@
       </c>
       <c r="E279" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8025,7 +8025,7 @@
       </c>
       <c r="E280" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8052,7 +8052,7 @@
       </c>
       <c r="E281" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8079,7 +8079,7 @@
       </c>
       <c r="E282" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8106,7 +8106,7 @@
       </c>
       <c r="E283" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8133,7 +8133,7 @@
       </c>
       <c r="E284" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8160,7 +8160,7 @@
       </c>
       <c r="E285" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8187,7 +8187,7 @@
       </c>
       <c r="E286" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8214,7 +8214,7 @@
       </c>
       <c r="E287" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8241,7 +8241,7 @@
       </c>
       <c r="E288" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8268,7 +8268,7 @@
       </c>
       <c r="E289" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8295,7 +8295,7 @@
       </c>
       <c r="E290" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8322,7 +8322,7 @@
       </c>
       <c r="E291" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8349,7 +8349,7 @@
       </c>
       <c r="E292" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8376,7 +8376,7 @@
       </c>
       <c r="E293" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8403,7 +8403,7 @@
       </c>
       <c r="E294" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8430,7 +8430,7 @@
       </c>
       <c r="E295" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8457,7 +8457,7 @@
       </c>
       <c r="E296" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8484,7 +8484,7 @@
       </c>
       <c r="E297" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8511,7 +8511,7 @@
       </c>
       <c r="E298" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8538,7 +8538,7 @@
       </c>
       <c r="E299" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8565,7 +8565,7 @@
       </c>
       <c r="E300" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8592,7 +8592,7 @@
       </c>
       <c r="E301" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8619,7 +8619,7 @@
       </c>
       <c r="E302" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8646,7 +8646,7 @@
       </c>
       <c r="E303" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8673,7 +8673,7 @@
       </c>
       <c r="E304" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8700,7 +8700,7 @@
       </c>
       <c r="E305" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8727,7 +8727,7 @@
       </c>
       <c r="E306" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8754,7 +8754,7 @@
       </c>
       <c r="E307" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8781,7 +8781,7 @@
       </c>
       <c r="E308" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8808,7 +8808,7 @@
       </c>
       <c r="E309" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8835,7 +8835,7 @@
       </c>
       <c r="E310" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8862,7 +8862,7 @@
       </c>
       <c r="E311" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8889,7 +8889,7 @@
       </c>
       <c r="E312" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8916,7 +8916,7 @@
       </c>
       <c r="E313" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8943,7 +8943,7 @@
       </c>
       <c r="E314" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8970,7 +8970,7 @@
       </c>
       <c r="E315" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -8997,7 +8997,7 @@
       </c>
       <c r="E316" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -9024,7 +9024,7 @@
       </c>
       <c r="E317" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -9051,7 +9051,7 @@
       </c>
       <c r="E318" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -9078,7 +9078,7 @@
       </c>
       <c r="E319" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>
@@ -9105,7 +9105,34 @@
       </c>
       <c r="E320" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" s="4" t="inlineStr">
+        <is>
+          <t>223007</t>
+        </is>
+      </c>
+      <c r="B321" s="4" t="inlineStr">
+        <is>
+          <t>خالد احمد محمد الكردى</t>
+        </is>
+      </c>
+      <c r="C321" s="4" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="D321" s="4" t="inlineStr">
+        <is>
+          <t>B1F2</t>
+        </is>
+      </c>
+      <c r="E321" s="4" t="inlineStr">
+        <is>
+          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Upload Y4_B2526_General_&_Special_Surgery_1_B1_reference_data.xlsx via attendance app
</commit_message>
<xml_diff>
--- a/reference_data/Y4_B2526_General_&_Special_Surgery_1_B1_reference_data.xlsx
+++ b/reference_data/Y4_B2526_General_&_Special_Surgery_1_B1_reference_data.xlsx
@@ -454,7 +454,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E321"/>
+  <dimension ref="A1:E322"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,7 +519,7 @@
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -546,7 +546,7 @@
       </c>
       <c r="E3" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -573,7 +573,7 @@
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -600,7 +600,7 @@
       </c>
       <c r="E5" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -627,7 +627,7 @@
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -654,7 +654,7 @@
       </c>
       <c r="E7" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -681,7 +681,7 @@
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -708,7 +708,7 @@
       </c>
       <c r="E9" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -735,7 +735,7 @@
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -762,7 +762,7 @@
       </c>
       <c r="E11" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -789,7 +789,7 @@
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -816,7 +816,7 @@
       </c>
       <c r="E13" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -843,7 +843,7 @@
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -870,7 +870,7 @@
       </c>
       <c r="E15" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -897,7 +897,7 @@
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -924,7 +924,7 @@
       </c>
       <c r="E17" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -951,7 +951,7 @@
       </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -978,7 +978,7 @@
       </c>
       <c r="E19" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1005,7 +1005,7 @@
       </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1032,7 +1032,7 @@
       </c>
       <c r="E21" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="E22" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1086,7 +1086,7 @@
       </c>
       <c r="E23" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1113,7 +1113,7 @@
       </c>
       <c r="E24" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1140,7 +1140,7 @@
       </c>
       <c r="E25" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1167,7 +1167,7 @@
       </c>
       <c r="E26" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1194,7 +1194,7 @@
       </c>
       <c r="E27" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1221,7 +1221,7 @@
       </c>
       <c r="E28" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1248,7 +1248,7 @@
       </c>
       <c r="E29" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1275,7 +1275,7 @@
       </c>
       <c r="E30" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1302,7 +1302,7 @@
       </c>
       <c r="E31" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1329,7 +1329,7 @@
       </c>
       <c r="E32" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1356,7 +1356,7 @@
       </c>
       <c r="E33" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1383,7 +1383,7 @@
       </c>
       <c r="E34" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1410,7 +1410,7 @@
       </c>
       <c r="E35" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1437,7 +1437,7 @@
       </c>
       <c r="E36" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1464,7 +1464,7 @@
       </c>
       <c r="E37" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1491,7 +1491,7 @@
       </c>
       <c r="E38" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1518,7 +1518,7 @@
       </c>
       <c r="E39" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="E40" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1572,7 +1572,7 @@
       </c>
       <c r="E41" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1599,7 +1599,7 @@
       </c>
       <c r="E42" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1626,7 +1626,7 @@
       </c>
       <c r="E43" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1653,7 +1653,7 @@
       </c>
       <c r="E44" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1680,7 +1680,7 @@
       </c>
       <c r="E45" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1707,7 +1707,7 @@
       </c>
       <c r="E46" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1734,7 +1734,7 @@
       </c>
       <c r="E47" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1761,7 +1761,7 @@
       </c>
       <c r="E48" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1788,7 +1788,7 @@
       </c>
       <c r="E49" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1815,7 +1815,7 @@
       </c>
       <c r="E50" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1842,7 +1842,7 @@
       </c>
       <c r="E51" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1869,7 +1869,7 @@
       </c>
       <c r="E52" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1896,7 +1896,7 @@
       </c>
       <c r="E53" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1923,7 +1923,7 @@
       </c>
       <c r="E54" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1950,7 +1950,7 @@
       </c>
       <c r="E55" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -1977,7 +1977,7 @@
       </c>
       <c r="E56" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2004,7 +2004,7 @@
       </c>
       <c r="E57" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2031,7 +2031,7 @@
       </c>
       <c r="E58" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2058,7 +2058,7 @@
       </c>
       <c r="E59" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2085,7 +2085,7 @@
       </c>
       <c r="E60" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2112,7 +2112,7 @@
       </c>
       <c r="E61" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2139,7 +2139,7 @@
       </c>
       <c r="E62" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2166,7 +2166,7 @@
       </c>
       <c r="E63" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2193,7 +2193,7 @@
       </c>
       <c r="E64" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2220,7 +2220,7 @@
       </c>
       <c r="E65" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2247,7 +2247,7 @@
       </c>
       <c r="E66" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2274,7 +2274,7 @@
       </c>
       <c r="E67" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2301,7 +2301,7 @@
       </c>
       <c r="E68" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2328,7 +2328,7 @@
       </c>
       <c r="E69" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2355,7 +2355,7 @@
       </c>
       <c r="E70" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2382,7 +2382,7 @@
       </c>
       <c r="E71" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2409,7 +2409,7 @@
       </c>
       <c r="E72" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2436,7 +2436,7 @@
       </c>
       <c r="E73" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2463,7 +2463,7 @@
       </c>
       <c r="E74" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2490,7 +2490,7 @@
       </c>
       <c r="E75" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2517,7 +2517,7 @@
       </c>
       <c r="E76" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2544,7 +2544,7 @@
       </c>
       <c r="E77" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2571,7 +2571,7 @@
       </c>
       <c r="E78" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2598,7 +2598,7 @@
       </c>
       <c r="E79" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2625,7 +2625,7 @@
       </c>
       <c r="E80" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2652,7 +2652,7 @@
       </c>
       <c r="E81" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2679,7 +2679,7 @@
       </c>
       <c r="E82" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2706,7 +2706,7 @@
       </c>
       <c r="E83" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2733,7 +2733,7 @@
       </c>
       <c r="E84" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2760,7 +2760,7 @@
       </c>
       <c r="E85" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2787,7 +2787,7 @@
       </c>
       <c r="E86" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2814,7 +2814,7 @@
       </c>
       <c r="E87" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2841,7 +2841,7 @@
       </c>
       <c r="E88" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2868,7 +2868,7 @@
       </c>
       <c r="E89" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2895,7 +2895,7 @@
       </c>
       <c r="E90" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2922,7 +2922,7 @@
       </c>
       <c r="E91" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2949,7 +2949,7 @@
       </c>
       <c r="E92" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -2976,7 +2976,7 @@
       </c>
       <c r="E93" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3003,7 +3003,7 @@
       </c>
       <c r="E94" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3030,7 +3030,7 @@
       </c>
       <c r="E95" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3057,7 +3057,7 @@
       </c>
       <c r="E96" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3084,7 +3084,7 @@
       </c>
       <c r="E97" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3111,7 +3111,7 @@
       </c>
       <c r="E98" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3138,7 +3138,7 @@
       </c>
       <c r="E99" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3165,7 +3165,7 @@
       </c>
       <c r="E100" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3192,7 +3192,7 @@
       </c>
       <c r="E101" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3219,7 +3219,7 @@
       </c>
       <c r="E102" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3246,7 +3246,7 @@
       </c>
       <c r="E103" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3273,7 +3273,7 @@
       </c>
       <c r="E104" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3300,7 +3300,7 @@
       </c>
       <c r="E105" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3327,7 +3327,7 @@
       </c>
       <c r="E106" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3354,7 +3354,7 @@
       </c>
       <c r="E107" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3381,7 +3381,7 @@
       </c>
       <c r="E108" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3408,7 +3408,7 @@
       </c>
       <c r="E109" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3435,7 +3435,7 @@
       </c>
       <c r="E110" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3462,7 +3462,7 @@
       </c>
       <c r="E111" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3489,7 +3489,7 @@
       </c>
       <c r="E112" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3516,7 +3516,7 @@
       </c>
       <c r="E113" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3543,7 +3543,7 @@
       </c>
       <c r="E114" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3570,7 +3570,7 @@
       </c>
       <c r="E115" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3597,7 +3597,7 @@
       </c>
       <c r="E116" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3624,7 +3624,7 @@
       </c>
       <c r="E117" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3651,7 +3651,7 @@
       </c>
       <c r="E118" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3678,7 +3678,7 @@
       </c>
       <c r="E119" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3705,7 +3705,7 @@
       </c>
       <c r="E120" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3732,7 +3732,7 @@
       </c>
       <c r="E121" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3759,7 +3759,7 @@
       </c>
       <c r="E122" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3786,7 +3786,7 @@
       </c>
       <c r="E123" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3813,7 +3813,7 @@
       </c>
       <c r="E124" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3840,7 +3840,7 @@
       </c>
       <c r="E125" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3867,7 +3867,7 @@
       </c>
       <c r="E126" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3894,7 +3894,7 @@
       </c>
       <c r="E127" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3921,7 +3921,7 @@
       </c>
       <c r="E128" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3948,7 +3948,7 @@
       </c>
       <c r="E129" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -3975,7 +3975,7 @@
       </c>
       <c r="E130" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4002,7 +4002,7 @@
       </c>
       <c r="E131" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4029,7 +4029,7 @@
       </c>
       <c r="E132" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4056,7 +4056,7 @@
       </c>
       <c r="E133" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4083,7 +4083,7 @@
       </c>
       <c r="E134" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4110,7 +4110,7 @@
       </c>
       <c r="E135" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4137,7 +4137,7 @@
       </c>
       <c r="E136" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4164,7 +4164,7 @@
       </c>
       <c r="E137" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4191,7 +4191,7 @@
       </c>
       <c r="E138" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4218,7 +4218,7 @@
       </c>
       <c r="E139" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4245,7 +4245,7 @@
       </c>
       <c r="E140" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4272,7 +4272,7 @@
       </c>
       <c r="E141" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4299,7 +4299,7 @@
       </c>
       <c r="E142" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4326,7 +4326,7 @@
       </c>
       <c r="E143" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4353,7 +4353,7 @@
       </c>
       <c r="E144" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4380,7 +4380,7 @@
       </c>
       <c r="E145" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4407,7 +4407,7 @@
       </c>
       <c r="E146" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4434,7 +4434,7 @@
       </c>
       <c r="E147" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4461,7 +4461,7 @@
       </c>
       <c r="E148" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4488,7 +4488,7 @@
       </c>
       <c r="E149" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4515,7 +4515,7 @@
       </c>
       <c r="E150" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4542,7 +4542,7 @@
       </c>
       <c r="E151" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4569,7 +4569,7 @@
       </c>
       <c r="E152" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4596,7 +4596,7 @@
       </c>
       <c r="E153" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4623,7 +4623,7 @@
       </c>
       <c r="E154" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4650,7 +4650,7 @@
       </c>
       <c r="E155" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4677,7 +4677,7 @@
       </c>
       <c r="E156" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4704,7 +4704,7 @@
       </c>
       <c r="E157" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4731,7 +4731,7 @@
       </c>
       <c r="E158" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4758,7 +4758,7 @@
       </c>
       <c r="E159" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4785,7 +4785,7 @@
       </c>
       <c r="E160" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4812,7 +4812,7 @@
       </c>
       <c r="E161" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4839,7 +4839,7 @@
       </c>
       <c r="E162" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4866,7 +4866,7 @@
       </c>
       <c r="E163" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4893,7 +4893,7 @@
       </c>
       <c r="E164" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4920,7 +4920,7 @@
       </c>
       <c r="E165" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4947,7 +4947,7 @@
       </c>
       <c r="E166" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -4974,7 +4974,7 @@
       </c>
       <c r="E167" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5001,7 +5001,7 @@
       </c>
       <c r="E168" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5028,7 +5028,7 @@
       </c>
       <c r="E169" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5055,7 +5055,7 @@
       </c>
       <c r="E170" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5082,7 +5082,7 @@
       </c>
       <c r="E171" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5109,7 +5109,7 @@
       </c>
       <c r="E172" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5136,7 +5136,7 @@
       </c>
       <c r="E173" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5163,7 +5163,7 @@
       </c>
       <c r="E174" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5190,7 +5190,7 @@
       </c>
       <c r="E175" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5217,7 +5217,7 @@
       </c>
       <c r="E176" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5244,7 +5244,7 @@
       </c>
       <c r="E177" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5271,7 +5271,7 @@
       </c>
       <c r="E178" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5298,7 +5298,7 @@
       </c>
       <c r="E179" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5325,7 +5325,7 @@
       </c>
       <c r="E180" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5352,7 +5352,7 @@
       </c>
       <c r="E181" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5379,7 +5379,7 @@
       </c>
       <c r="E182" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5406,7 +5406,7 @@
       </c>
       <c r="E183" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5433,7 +5433,7 @@
       </c>
       <c r="E184" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5460,7 +5460,7 @@
       </c>
       <c r="E185" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5487,7 +5487,7 @@
       </c>
       <c r="E186" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5514,7 +5514,7 @@
       </c>
       <c r="E187" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5541,7 +5541,7 @@
       </c>
       <c r="E188" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5568,7 +5568,7 @@
       </c>
       <c r="E189" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5595,7 +5595,7 @@
       </c>
       <c r="E190" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5622,7 +5622,7 @@
       </c>
       <c r="E191" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5649,7 +5649,7 @@
       </c>
       <c r="E192" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5676,7 +5676,7 @@
       </c>
       <c r="E193" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5703,7 +5703,7 @@
       </c>
       <c r="E194" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5730,7 +5730,7 @@
       </c>
       <c r="E195" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5757,7 +5757,7 @@
       </c>
       <c r="E196" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5784,7 +5784,7 @@
       </c>
       <c r="E197" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5811,7 +5811,7 @@
       </c>
       <c r="E198" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5838,7 +5838,7 @@
       </c>
       <c r="E199" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5865,7 +5865,7 @@
       </c>
       <c r="E200" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5892,7 +5892,7 @@
       </c>
       <c r="E201" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5919,7 +5919,7 @@
       </c>
       <c r="E202" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5946,7 +5946,7 @@
       </c>
       <c r="E203" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -5973,7 +5973,7 @@
       </c>
       <c r="E204" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -6000,7 +6000,7 @@
       </c>
       <c r="E205" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -6027,7 +6027,7 @@
       </c>
       <c r="E206" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -6054,7 +6054,7 @@
       </c>
       <c r="E207" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -6081,7 +6081,7 @@
       </c>
       <c r="E208" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -6108,7 +6108,7 @@
       </c>
       <c r="E209" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -6135,7 +6135,7 @@
       </c>
       <c r="E210" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -6162,7 +6162,7 @@
       </c>
       <c r="E211" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -6189,7 +6189,7 @@
       </c>
       <c r="E212" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -6216,7 +6216,7 @@
       </c>
       <c r="E213" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -6243,7 +6243,7 @@
       </c>
       <c r="E214" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -6270,7 +6270,7 @@
       </c>
       <c r="E215" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -6297,7 +6297,7 @@
       </c>
       <c r="E216" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -6324,7 +6324,7 @@
       </c>
       <c r="E217" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -6351,7 +6351,7 @@
       </c>
       <c r="E218" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -6378,7 +6378,7 @@
       </c>
       <c r="E219" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -6405,7 +6405,7 @@
       </c>
       <c r="E220" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
@@ -6432,19 +6432,19 @@
       </c>
       <c r="E221" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="3" t="inlineStr">
         <is>
-          <t>221936</t>
+          <t>221908</t>
         </is>
       </c>
       <c r="B222" s="3" t="inlineStr">
         <is>
-          <t>كنان عبد الرحمن الاحمد الرويلي</t>
+          <t>أحمد معتز احمد محمد الامين</t>
         </is>
       </c>
       <c r="C222" s="3" t="inlineStr">
@@ -6459,19 +6459,19 @@
       </c>
       <c r="E222" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="4" t="inlineStr">
         <is>
-          <t>221939</t>
+          <t>221936</t>
         </is>
       </c>
       <c r="B223" s="4" t="inlineStr">
         <is>
-          <t>لبنى محمد الحاج عباس ابنعوف</t>
+          <t>كنان عبد الرحمن الاحمد الرويلي</t>
         </is>
       </c>
       <c r="C223" s="4" t="inlineStr">
@@ -6486,19 +6486,19 @@
       </c>
       <c r="E223" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="3" t="inlineStr">
         <is>
-          <t>221956</t>
+          <t>221939</t>
         </is>
       </c>
       <c r="B224" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">خالد محمد ترياقى </t>
+          <t>لبنى محمد الحاج عباس ابنعوف</t>
         </is>
       </c>
       <c r="C224" s="3" t="inlineStr">
@@ -6513,19 +6513,19 @@
       </c>
       <c r="E224" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="4" t="inlineStr">
         <is>
-          <t>221957</t>
+          <t>221956</t>
         </is>
       </c>
       <c r="B225" s="4" t="inlineStr">
         <is>
-          <t>باسل احمد محمد احمد</t>
+          <t xml:space="preserve">خالد محمد ترياقى </t>
         </is>
       </c>
       <c r="C225" s="4" t="inlineStr">
@@ -6540,19 +6540,19 @@
       </c>
       <c r="E225" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="3" t="inlineStr">
         <is>
-          <t>221961</t>
+          <t>221957</t>
         </is>
       </c>
       <c r="B226" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">ياسمين بابكر موسى بابكر </t>
+          <t>باسل احمد محمد احمد</t>
         </is>
       </c>
       <c r="C226" s="3" t="inlineStr">
@@ -6567,19 +6567,19 @@
       </c>
       <c r="E226" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="4" t="inlineStr">
         <is>
-          <t>221967</t>
+          <t>221961</t>
         </is>
       </c>
       <c r="B227" s="4" t="inlineStr">
         <is>
-          <t>حسن اسماعيل اشحيبر</t>
+          <t xml:space="preserve">ياسمين بابكر موسى بابكر </t>
         </is>
       </c>
       <c r="C227" s="4" t="inlineStr">
@@ -6594,19 +6594,19 @@
       </c>
       <c r="E227" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="3" t="inlineStr">
         <is>
-          <t>221974</t>
+          <t>221967</t>
         </is>
       </c>
       <c r="B228" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">ابرار كمال محمد عمر </t>
+          <t>حسن اسماعيل اشحيبر</t>
         </is>
       </c>
       <c r="C228" s="3" t="inlineStr">
@@ -6621,19 +6621,19 @@
       </c>
       <c r="E228" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="4" t="inlineStr">
         <is>
-          <t>221994</t>
+          <t>221974</t>
         </is>
       </c>
       <c r="B229" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">رنا محمد مصطفى على </t>
+          <t xml:space="preserve">ابرار كمال محمد عمر </t>
         </is>
       </c>
       <c r="C229" s="4" t="inlineStr">
@@ -6648,19 +6648,19 @@
       </c>
       <c r="E229" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="3" t="inlineStr">
         <is>
-          <t>221999</t>
+          <t>221994</t>
         </is>
       </c>
       <c r="B230" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">منذر عبد الله بلال مضوى </t>
+          <t xml:space="preserve">رنا محمد مصطفى على </t>
         </is>
       </c>
       <c r="C230" s="3" t="inlineStr">
@@ -6675,19 +6675,19 @@
       </c>
       <c r="E230" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="4" t="inlineStr">
         <is>
-          <t>222009</t>
+          <t>221999</t>
         </is>
       </c>
       <c r="B231" s="4" t="inlineStr">
         <is>
-          <t>حسن عبد العزيز حسن عبد المجيد</t>
+          <t xml:space="preserve">منذر عبد الله بلال مضوى </t>
         </is>
       </c>
       <c r="C231" s="4" t="inlineStr">
@@ -6702,19 +6702,19 @@
       </c>
       <c r="E231" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="3" t="inlineStr">
         <is>
-          <t>222048</t>
+          <t>222009</t>
         </is>
       </c>
       <c r="B232" s="3" t="inlineStr">
         <is>
-          <t>المعتصم بالله مصطفى محمد على</t>
+          <t>حسن عبد العزيز حسن عبد المجيد</t>
         </is>
       </c>
       <c r="C232" s="3" t="inlineStr">
@@ -6729,19 +6729,19 @@
       </c>
       <c r="E232" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="4" t="inlineStr">
         <is>
-          <t>222050</t>
+          <t>222048</t>
         </is>
       </c>
       <c r="B233" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">هاجر طة عبد الحميد طه </t>
+          <t>المعتصم بالله مصطفى محمد على</t>
         </is>
       </c>
       <c r="C233" s="4" t="inlineStr">
@@ -6756,19 +6756,19 @@
       </c>
       <c r="E233" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="3" t="inlineStr">
         <is>
-          <t>222060</t>
+          <t>222050</t>
         </is>
       </c>
       <c r="B234" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">عثمان عبد الخالق عثمان عبده </t>
+          <t xml:space="preserve">هاجر طة عبد الحميد طه </t>
         </is>
       </c>
       <c r="C234" s="3" t="inlineStr">
@@ -6783,19 +6783,19 @@
       </c>
       <c r="E234" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="4" t="inlineStr">
         <is>
-          <t>222062</t>
+          <t>222060</t>
         </is>
       </c>
       <c r="B235" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">محمد المصطفى ادم داؤد على </t>
+          <t xml:space="preserve">عثمان عبد الخالق عثمان عبده </t>
         </is>
       </c>
       <c r="C235" s="4" t="inlineStr">
@@ -6810,19 +6810,19 @@
       </c>
       <c r="E235" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="3" t="inlineStr">
         <is>
-          <t>222064</t>
+          <t>222062</t>
         </is>
       </c>
       <c r="B236" s="3" t="inlineStr">
         <is>
-          <t>ميسره احمد عمر احمد</t>
+          <t xml:space="preserve">محمد المصطفى ادم داؤد على </t>
         </is>
       </c>
       <c r="C236" s="3" t="inlineStr">
@@ -6837,19 +6837,19 @@
       </c>
       <c r="E236" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="4" t="inlineStr">
         <is>
-          <t>222075</t>
+          <t>222064</t>
         </is>
       </c>
       <c r="B237" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">النذير احمد داؤد اسو  </t>
+          <t>ميسره احمد عمر احمد</t>
         </is>
       </c>
       <c r="C237" s="4" t="inlineStr">
@@ -6864,19 +6864,19 @@
       </c>
       <c r="E237" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="3" t="inlineStr">
         <is>
-          <t>222078</t>
+          <t>222075</t>
         </is>
       </c>
       <c r="B238" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">صهيب عبد المنعم طه عثمان </t>
+          <t xml:space="preserve">النذير احمد داؤد اسو  </t>
         </is>
       </c>
       <c r="C238" s="3" t="inlineStr">
@@ -6891,19 +6891,19 @@
       </c>
       <c r="E238" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="4" t="inlineStr">
         <is>
-          <t>210288</t>
+          <t>222078</t>
         </is>
       </c>
       <c r="B239" s="4" t="inlineStr">
         <is>
-          <t>عمرو اشرف جابر رمضان</t>
+          <t xml:space="preserve">صهيب عبد المنعم طه عثمان </t>
         </is>
       </c>
       <c r="C239" s="4" t="inlineStr">
@@ -6913,24 +6913,24 @@
       </c>
       <c r="D239" s="4" t="inlineStr">
         <is>
-          <t>B1E2</t>
+          <t>B1E1</t>
         </is>
       </c>
       <c r="E239" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="3" t="inlineStr">
         <is>
-          <t>210301</t>
+          <t>210288</t>
         </is>
       </c>
       <c r="B240" s="3" t="inlineStr">
         <is>
-          <t>ابانوب ايمن جميل وديع</t>
+          <t>عمرو اشرف جابر رمضان</t>
         </is>
       </c>
       <c r="C240" s="3" t="inlineStr">
@@ -6945,19 +6945,19 @@
       </c>
       <c r="E240" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="4" t="inlineStr">
         <is>
-          <t>210306</t>
+          <t>210301</t>
         </is>
       </c>
       <c r="B241" s="4" t="inlineStr">
         <is>
-          <t>احمد اشرف احمد رجب غزال</t>
+          <t>ابانوب ايمن جميل وديع</t>
         </is>
       </c>
       <c r="C241" s="4" t="inlineStr">
@@ -6972,19 +6972,19 @@
       </c>
       <c r="E241" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="3" t="inlineStr">
         <is>
-          <t>210319</t>
+          <t>210306</t>
         </is>
       </c>
       <c r="B242" s="3" t="inlineStr">
         <is>
-          <t>احمد سامح جمعه عبد المجيد محمد</t>
+          <t>احمد اشرف احمد رجب غزال</t>
         </is>
       </c>
       <c r="C242" s="3" t="inlineStr">
@@ -6999,19 +6999,19 @@
       </c>
       <c r="E242" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="4" t="inlineStr">
         <is>
-          <t>210333</t>
+          <t>210319</t>
         </is>
       </c>
       <c r="B243" s="4" t="inlineStr">
         <is>
-          <t>احمد محمد عبد الجواد مندور هاشم</t>
+          <t>احمد سامح جمعه عبد المجيد محمد</t>
         </is>
       </c>
       <c r="C243" s="4" t="inlineStr">
@@ -7026,19 +7026,19 @@
       </c>
       <c r="E243" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="3" t="inlineStr">
         <is>
-          <t>210334</t>
+          <t>210333</t>
         </is>
       </c>
       <c r="B244" s="3" t="inlineStr">
         <is>
-          <t>احمد محمد عبد المجيد عبد العاطي</t>
+          <t>احمد محمد عبد الجواد مندور هاشم</t>
         </is>
       </c>
       <c r="C244" s="3" t="inlineStr">
@@ -7053,19 +7053,19 @@
       </c>
       <c r="E244" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="4" t="inlineStr">
         <is>
-          <t>210340</t>
+          <t>210334</t>
         </is>
       </c>
       <c r="B245" s="4" t="inlineStr">
         <is>
-          <t>احمد منتصر سيد منتصر احمد</t>
+          <t>احمد محمد عبد المجيد عبد العاطي</t>
         </is>
       </c>
       <c r="C245" s="4" t="inlineStr">
@@ -7080,19 +7080,19 @@
       </c>
       <c r="E245" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="3" t="inlineStr">
         <is>
-          <t>210354</t>
+          <t>210340</t>
         </is>
       </c>
       <c r="B246" s="3" t="inlineStr">
         <is>
-          <t>اسراء حسني مصطفى احمد</t>
+          <t>احمد منتصر سيد منتصر احمد</t>
         </is>
       </c>
       <c r="C246" s="3" t="inlineStr">
@@ -7107,19 +7107,19 @@
       </c>
       <c r="E246" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="4" t="inlineStr">
         <is>
-          <t>210385</t>
+          <t>210354</t>
         </is>
       </c>
       <c r="B247" s="4" t="inlineStr">
         <is>
-          <t>ايمان طارق مصطفى سيد احمد</t>
+          <t>اسراء حسني مصطفى احمد</t>
         </is>
       </c>
       <c r="C247" s="4" t="inlineStr">
@@ -7134,19 +7134,19 @@
       </c>
       <c r="E247" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="3" t="inlineStr">
         <is>
-          <t>210387</t>
+          <t>210385</t>
         </is>
       </c>
       <c r="B248" s="3" t="inlineStr">
         <is>
-          <t>ايمان محمد يوسف محمد</t>
+          <t>ايمان طارق مصطفى سيد احمد</t>
         </is>
       </c>
       <c r="C248" s="3" t="inlineStr">
@@ -7161,19 +7161,19 @@
       </c>
       <c r="E248" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="4" t="inlineStr">
         <is>
-          <t>210401</t>
+          <t>210387</t>
         </is>
       </c>
       <c r="B249" s="4" t="inlineStr">
         <is>
-          <t>بافلى عماد غبريال مترى</t>
+          <t>ايمان محمد يوسف محمد</t>
         </is>
       </c>
       <c r="C249" s="4" t="inlineStr">
@@ -7188,19 +7188,19 @@
       </c>
       <c r="E249" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="3" t="inlineStr">
         <is>
-          <t>210421</t>
+          <t>210401</t>
         </is>
       </c>
       <c r="B250" s="3" t="inlineStr">
         <is>
-          <t>توماس مرجان فوزى شكر الله</t>
+          <t>بافلى عماد غبريال مترى</t>
         </is>
       </c>
       <c r="C250" s="3" t="inlineStr">
@@ -7215,19 +7215,19 @@
       </c>
       <c r="E250" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="4" t="inlineStr">
         <is>
-          <t>210435</t>
+          <t>210421</t>
         </is>
       </c>
       <c r="B251" s="4" t="inlineStr">
         <is>
-          <t>حسن محمد حسن مرسى</t>
+          <t>توماس مرجان فوزى شكر الله</t>
         </is>
       </c>
       <c r="C251" s="4" t="inlineStr">
@@ -7242,19 +7242,19 @@
       </c>
       <c r="E251" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="3" t="inlineStr">
         <is>
-          <t>210438</t>
+          <t>210435</t>
         </is>
       </c>
       <c r="B252" s="3" t="inlineStr">
         <is>
-          <t>حسينى طارق حسينى محمد الطويل</t>
+          <t>حسن محمد حسن مرسى</t>
         </is>
       </c>
       <c r="C252" s="3" t="inlineStr">
@@ -7269,19 +7269,19 @@
       </c>
       <c r="E252" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="4" t="inlineStr">
         <is>
-          <t>221582</t>
+          <t>210438</t>
         </is>
       </c>
       <c r="B253" s="4" t="inlineStr">
         <is>
-          <t>شهد صلاح جعفر الشيخ ادريس</t>
+          <t>حسينى طارق حسينى محمد الطويل</t>
         </is>
       </c>
       <c r="C253" s="4" t="inlineStr">
@@ -7296,19 +7296,19 @@
       </c>
       <c r="E253" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="3" t="inlineStr">
         <is>
-          <t>222080</t>
+          <t>221582</t>
         </is>
       </c>
       <c r="B254" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">عبد الرحمن اسد الله حامد احمد </t>
+          <t>شهد صلاح جعفر الشيخ ادريس</t>
         </is>
       </c>
       <c r="C254" s="3" t="inlineStr">
@@ -7323,19 +7323,19 @@
       </c>
       <c r="E254" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="4" t="inlineStr">
         <is>
-          <t>222081</t>
+          <t>222080</t>
         </is>
       </c>
       <c r="B255" s="4" t="inlineStr">
         <is>
-          <t>عفيف عبد الجبار العبيد الصديق</t>
+          <t xml:space="preserve">عبد الرحمن اسد الله حامد احمد </t>
         </is>
       </c>
       <c r="C255" s="4" t="inlineStr">
@@ -7350,19 +7350,19 @@
       </c>
       <c r="E255" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="3" t="inlineStr">
         <is>
-          <t>222083</t>
+          <t>222081</t>
         </is>
       </c>
       <c r="B256" s="3" t="inlineStr">
         <is>
-          <t>محمد المجتبى فخر الدين بلال خليل</t>
+          <t>عفيف عبد الجبار العبيد الصديق</t>
         </is>
       </c>
       <c r="C256" s="3" t="inlineStr">
@@ -7377,19 +7377,19 @@
       </c>
       <c r="E256" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="4" t="inlineStr">
         <is>
-          <t>222085</t>
+          <t>222083</t>
         </is>
       </c>
       <c r="B257" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">مهند معاوية صالح جقدولة </t>
+          <t>محمد المجتبى فخر الدين بلال خليل</t>
         </is>
       </c>
       <c r="C257" s="4" t="inlineStr">
@@ -7404,19 +7404,19 @@
       </c>
       <c r="E257" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="3" t="inlineStr">
         <is>
-          <t>222089</t>
+          <t>222085</t>
         </is>
       </c>
       <c r="B258" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">نزار باسل عبد السميع جوده </t>
+          <t xml:space="preserve">مهند معاوية صالح جقدولة </t>
         </is>
       </c>
       <c r="C258" s="3" t="inlineStr">
@@ -7431,19 +7431,19 @@
       </c>
       <c r="E258" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="4" t="inlineStr">
         <is>
-          <t>222091</t>
+          <t>222089</t>
         </is>
       </c>
       <c r="B259" s="4" t="inlineStr">
         <is>
-          <t>سالم فايز سالم البلوى</t>
+          <t xml:space="preserve">نزار باسل عبد السميع جوده </t>
         </is>
       </c>
       <c r="C259" s="4" t="inlineStr">
@@ -7458,19 +7458,19 @@
       </c>
       <c r="E259" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="3" t="inlineStr">
         <is>
-          <t>222094</t>
+          <t>222091</t>
         </is>
       </c>
       <c r="B260" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">كريم برعى مكى برعى </t>
+          <t>سالم فايز سالم البلوى</t>
         </is>
       </c>
       <c r="C260" s="3" t="inlineStr">
@@ -7485,19 +7485,19 @@
       </c>
       <c r="E260" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="4" t="inlineStr">
         <is>
-          <t>222096</t>
+          <t>222094</t>
         </is>
       </c>
       <c r="B261" s="4" t="inlineStr">
         <is>
-          <t>محمود النميرى محمود ابراهيم</t>
+          <t xml:space="preserve">كريم برعى مكى برعى </t>
         </is>
       </c>
       <c r="C261" s="4" t="inlineStr">
@@ -7512,19 +7512,19 @@
       </c>
       <c r="E261" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="3" t="inlineStr">
         <is>
-          <t>222098</t>
+          <t>222096</t>
         </is>
       </c>
       <c r="B262" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">نعم عمر محمد عثمان </t>
+          <t>محمود النميرى محمود ابراهيم</t>
         </is>
       </c>
       <c r="C262" s="3" t="inlineStr">
@@ -7539,19 +7539,19 @@
       </c>
       <c r="E262" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="4" t="inlineStr">
         <is>
-          <t>222102</t>
+          <t>222098</t>
         </is>
       </c>
       <c r="B263" s="4" t="inlineStr">
         <is>
-          <t>محمد حسن حمدو حسن</t>
+          <t xml:space="preserve">نعم عمر محمد عثمان </t>
         </is>
       </c>
       <c r="C263" s="4" t="inlineStr">
@@ -7566,19 +7566,19 @@
       </c>
       <c r="E263" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="3" t="inlineStr">
         <is>
-          <t>222106</t>
+          <t>222102</t>
         </is>
       </c>
       <c r="B264" s="3" t="inlineStr">
         <is>
-          <t>عمرو ياسر عثمان عبد المجيد</t>
+          <t>محمد حسن حمدو حسن</t>
         </is>
       </c>
       <c r="C264" s="3" t="inlineStr">
@@ -7593,19 +7593,19 @@
       </c>
       <c r="E264" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="4" t="inlineStr">
         <is>
-          <t>222111</t>
+          <t>222106</t>
         </is>
       </c>
       <c r="B265" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">ليازيا الفاتح صالح ادريس </t>
+          <t>عمرو ياسر عثمان عبد المجيد</t>
         </is>
       </c>
       <c r="C265" s="4" t="inlineStr">
@@ -7620,19 +7620,19 @@
       </c>
       <c r="E265" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="3" t="inlineStr">
         <is>
-          <t>222123</t>
+          <t>222111</t>
         </is>
       </c>
       <c r="B266" s="3" t="inlineStr">
         <is>
-          <t>عبد الله العوض سليمان بابكر</t>
+          <t xml:space="preserve">ليازيا الفاتح صالح ادريس </t>
         </is>
       </c>
       <c r="C266" s="3" t="inlineStr">
@@ -7647,19 +7647,19 @@
       </c>
       <c r="E266" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="4" t="inlineStr">
         <is>
-          <t>210509</t>
+          <t>222123</t>
         </is>
       </c>
       <c r="B267" s="4" t="inlineStr">
         <is>
-          <t>شروق محمود محمد محمود فرحات</t>
+          <t>عبد الله العوض سليمان بابكر</t>
         </is>
       </c>
       <c r="C267" s="4" t="inlineStr">
@@ -7669,24 +7669,24 @@
       </c>
       <c r="D267" s="4" t="inlineStr">
         <is>
-          <t>B1F1</t>
+          <t>B1E2</t>
         </is>
       </c>
       <c r="E267" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="3" t="inlineStr">
         <is>
-          <t>210513</t>
+          <t>210509</t>
         </is>
       </c>
       <c r="B268" s="3" t="inlineStr">
         <is>
-          <t>شهد عبد الرحمن احمد الشاذلى</t>
+          <t>شروق محمود محمد محمود فرحات</t>
         </is>
       </c>
       <c r="C268" s="3" t="inlineStr">
@@ -7701,19 +7701,19 @@
       </c>
       <c r="E268" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="4" t="inlineStr">
         <is>
-          <t>210516</t>
+          <t>210513</t>
         </is>
       </c>
       <c r="B269" s="4" t="inlineStr">
         <is>
-          <t>شرين سيف النصر</t>
+          <t>شهد عبد الرحمن احمد الشاذلى</t>
         </is>
       </c>
       <c r="C269" s="4" t="inlineStr">
@@ -7728,19 +7728,19 @@
       </c>
       <c r="E269" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="3" t="inlineStr">
         <is>
-          <t>210558</t>
+          <t>210516</t>
         </is>
       </c>
       <c r="B270" s="3" t="inlineStr">
         <is>
-          <t>على عبد الرؤف محمد بكرى</t>
+          <t>شرين سيف النصر</t>
         </is>
       </c>
       <c r="C270" s="3" t="inlineStr">
@@ -7755,19 +7755,19 @@
       </c>
       <c r="E270" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="4" t="inlineStr">
         <is>
-          <t>210621</t>
+          <t>210558</t>
         </is>
       </c>
       <c r="B271" s="4" t="inlineStr">
         <is>
-          <t>محمد رجب عبد المرضى سيد احمد عامر</t>
+          <t>على عبد الرؤف محمد بكرى</t>
         </is>
       </c>
       <c r="C271" s="4" t="inlineStr">
@@ -7782,19 +7782,19 @@
       </c>
       <c r="E271" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="3" t="inlineStr">
         <is>
-          <t>210686</t>
+          <t>210621</t>
         </is>
       </c>
       <c r="B272" s="3" t="inlineStr">
         <is>
-          <t>مصطفى ممدوح محمد ابو مسلم الصادق نصر</t>
+          <t>محمد رجب عبد المرضى سيد احمد عامر</t>
         </is>
       </c>
       <c r="C272" s="3" t="inlineStr">
@@ -7809,19 +7809,19 @@
       </c>
       <c r="E272" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="4" t="inlineStr">
         <is>
-          <t>210703</t>
+          <t>210686</t>
         </is>
       </c>
       <c r="B273" s="4" t="inlineStr">
         <is>
-          <t>منى ذو الهمه محمد الطبلاوى غنيم</t>
+          <t>مصطفى ممدوح محمد ابو مسلم الصادق نصر</t>
         </is>
       </c>
       <c r="C273" s="4" t="inlineStr">
@@ -7836,19 +7836,19 @@
       </c>
       <c r="E273" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="3" t="inlineStr">
         <is>
-          <t>210727</t>
+          <t>210703</t>
         </is>
       </c>
       <c r="B274" s="3" t="inlineStr">
         <is>
-          <t>ندى احمد عبد الله احمد عبد المجيد</t>
+          <t>منى ذو الهمه محمد الطبلاوى غنيم</t>
         </is>
       </c>
       <c r="C274" s="3" t="inlineStr">
@@ -7863,19 +7863,19 @@
       </c>
       <c r="E274" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="4" t="inlineStr">
         <is>
-          <t>210762</t>
+          <t>210727</t>
         </is>
       </c>
       <c r="B275" s="4" t="inlineStr">
         <is>
-          <t>هند السيد محمد السعيد سيد احمد</t>
+          <t>ندى احمد عبد الله احمد عبد المجيد</t>
         </is>
       </c>
       <c r="C275" s="4" t="inlineStr">
@@ -7890,19 +7890,19 @@
       </c>
       <c r="E275" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="3" t="inlineStr">
         <is>
-          <t>210799</t>
+          <t>210762</t>
         </is>
       </c>
       <c r="B276" s="3" t="inlineStr">
         <is>
-          <t>حسن ممدوح حسن صغير</t>
+          <t>هند السيد محمد السعيد سيد احمد</t>
         </is>
       </c>
       <c r="C276" s="3" t="inlineStr">
@@ -7917,19 +7917,19 @@
       </c>
       <c r="E276" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="4" t="inlineStr">
         <is>
-          <t>210809</t>
+          <t>210799</t>
         </is>
       </c>
       <c r="B277" s="4" t="inlineStr">
         <is>
-          <t>خطاب خالد هادى الوادعى</t>
+          <t>حسن ممدوح حسن صغير</t>
         </is>
       </c>
       <c r="C277" s="4" t="inlineStr">
@@ -7944,19 +7944,19 @@
       </c>
       <c r="E277" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="3" t="inlineStr">
         <is>
-          <t>210828</t>
+          <t>210809</t>
         </is>
       </c>
       <c r="B278" s="3" t="inlineStr">
         <is>
-          <t>Manal Hamid Nour Mahamat Terab</t>
+          <t>خطاب خالد هادى الوادعى</t>
         </is>
       </c>
       <c r="C278" s="3" t="inlineStr">
@@ -7971,19 +7971,19 @@
       </c>
       <c r="E278" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="4" t="inlineStr">
         <is>
-          <t>210832</t>
+          <t>210828</t>
         </is>
       </c>
       <c r="B279" s="4" t="inlineStr">
         <is>
-          <t>عصام الدين عادل محمد على</t>
+          <t>Manal Hamid Nour Mahamat Terab</t>
         </is>
       </c>
       <c r="C279" s="4" t="inlineStr">
@@ -7998,19 +7998,19 @@
       </c>
       <c r="E279" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="3" t="inlineStr">
         <is>
-          <t>210836</t>
+          <t>210832</t>
         </is>
       </c>
       <c r="B280" s="3" t="inlineStr">
         <is>
-          <t>عمه ديد درار</t>
+          <t>عصام الدين عادل محمد على</t>
         </is>
       </c>
       <c r="C280" s="3" t="inlineStr">
@@ -8025,19 +8025,19 @@
       </c>
       <c r="E280" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="4" t="inlineStr">
         <is>
-          <t>210839</t>
+          <t>210836</t>
         </is>
       </c>
       <c r="B281" s="4" t="inlineStr">
         <is>
-          <t>شكرى محمد حاد</t>
+          <t>نعمه دبد درار</t>
         </is>
       </c>
       <c r="C281" s="4" t="inlineStr">
@@ -8052,19 +8052,19 @@
       </c>
       <c r="E281" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="3" t="inlineStr">
         <is>
-          <t>210858</t>
+          <t>210839</t>
         </is>
       </c>
       <c r="B282" s="3" t="inlineStr">
         <is>
-          <t>محمد ابراهيم احمد عرجه</t>
+          <t>شكرى محمد حاد</t>
         </is>
       </c>
       <c r="C282" s="3" t="inlineStr">
@@ -8079,19 +8079,19 @@
       </c>
       <c r="E282" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="4" t="inlineStr">
         <is>
-          <t>210880</t>
+          <t>210858</t>
         </is>
       </c>
       <c r="B283" s="4" t="inlineStr">
         <is>
-          <t>نور الهدى ماجد عبد الامير</t>
+          <t>محمد ابراهيم احمد عرجه</t>
         </is>
       </c>
       <c r="C283" s="4" t="inlineStr">
@@ -8106,19 +8106,19 @@
       </c>
       <c r="E283" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="3" t="inlineStr">
         <is>
-          <t>210883</t>
+          <t>210880</t>
         </is>
       </c>
       <c r="B284" s="3" t="inlineStr">
         <is>
-          <t>احمد صلاح الدين عابدين صالح</t>
+          <t>نور الهدى ماجد عبد الامير</t>
         </is>
       </c>
       <c r="C284" s="3" t="inlineStr">
@@ -8133,19 +8133,19 @@
       </c>
       <c r="E284" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="4" t="inlineStr">
         <is>
-          <t>210887</t>
+          <t>210883</t>
         </is>
       </c>
       <c r="B285" s="4" t="inlineStr">
         <is>
-          <t>احمد عبد الله عبد القادر محمد</t>
+          <t>احمد صلاح الدين عابدين صالح</t>
         </is>
       </c>
       <c r="C285" s="4" t="inlineStr">
@@ -8160,19 +8160,19 @@
       </c>
       <c r="E285" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="3" t="inlineStr">
         <is>
-          <t>210892</t>
+          <t>210887</t>
         </is>
       </c>
       <c r="B286" s="3" t="inlineStr">
         <is>
-          <t>Yusof Barghouty</t>
+          <t>احمد عبد الله عبد القادر محمد</t>
         </is>
       </c>
       <c r="C286" s="3" t="inlineStr">
@@ -8187,19 +8187,19 @@
       </c>
       <c r="E286" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="4" t="inlineStr">
         <is>
-          <t>210902</t>
+          <t>210892</t>
         </is>
       </c>
       <c r="B287" s="4" t="inlineStr">
         <is>
-          <t>عبير ميسره محى الدين قاسم</t>
+          <t>Yusof Barghouty</t>
         </is>
       </c>
       <c r="C287" s="4" t="inlineStr">
@@ -8214,19 +8214,19 @@
       </c>
       <c r="E287" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="3" t="inlineStr">
         <is>
-          <t>210905</t>
+          <t>210902</t>
         </is>
       </c>
       <c r="B288" s="3" t="inlineStr">
         <is>
-          <t>ايمن خالد خليل الرجوب</t>
+          <t>عبير ميسره محى الدين قاسم</t>
         </is>
       </c>
       <c r="C288" s="3" t="inlineStr">
@@ -8241,19 +8241,19 @@
       </c>
       <c r="E288" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="4" t="inlineStr">
         <is>
-          <t>210910</t>
+          <t>210905</t>
         </is>
       </c>
       <c r="B289" s="4" t="inlineStr">
         <is>
-          <t>ابو بكر عبد الرحيم سنجك محمد</t>
+          <t>ايمن خالد خليل الرجوب</t>
         </is>
       </c>
       <c r="C289" s="4" t="inlineStr">
@@ -8268,19 +8268,19 @@
       </c>
       <c r="E289" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="3" t="inlineStr">
         <is>
-          <t>210921</t>
+          <t>210910</t>
         </is>
       </c>
       <c r="B290" s="3" t="inlineStr">
         <is>
-          <t>براء علاء محمد البيوك</t>
+          <t>ابو بكر عبد الرحيم سنجك محمد</t>
         </is>
       </c>
       <c r="C290" s="3" t="inlineStr">
@@ -8295,19 +8295,19 @@
       </c>
       <c r="E290" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="4" t="inlineStr">
         <is>
-          <t>210927</t>
+          <t>210921</t>
         </is>
       </c>
       <c r="B291" s="4" t="inlineStr">
         <is>
-          <t>ايمان فؤاد حامد ابو حمره</t>
+          <t>براء علاء محمد البيوك</t>
         </is>
       </c>
       <c r="C291" s="4" t="inlineStr">
@@ -8322,19 +8322,19 @@
       </c>
       <c r="E291" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="3" t="inlineStr">
         <is>
-          <t>210937</t>
+          <t>210927</t>
         </is>
       </c>
       <c r="B292" s="3" t="inlineStr">
         <is>
-          <t>عبد العزيز ناصر الجهمانى</t>
+          <t>ايمان فؤاد حامد ابو حمره</t>
         </is>
       </c>
       <c r="C292" s="3" t="inlineStr">
@@ -8349,19 +8349,19 @@
       </c>
       <c r="E292" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="4" t="inlineStr">
         <is>
-          <t>201577</t>
+          <t>210937</t>
         </is>
       </c>
       <c r="B293" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> عزام عبد الله على حسن الحكمى</t>
+          <t>عبد العزيز ناصر الجهمانى</t>
         </is>
       </c>
       <c r="C293" s="4" t="inlineStr">
@@ -8371,24 +8371,24 @@
       </c>
       <c r="D293" s="4" t="inlineStr">
         <is>
-          <t>B1F2</t>
+          <t>B1F1</t>
         </is>
       </c>
       <c r="E293" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="3" t="inlineStr">
         <is>
-          <t>210840</t>
+          <t>201577</t>
         </is>
       </c>
       <c r="B294" s="3" t="inlineStr">
         <is>
-          <t>يونس دينى اسماعيل</t>
+          <t xml:space="preserve"> عزام عبد الله على حسن الحكمى</t>
         </is>
       </c>
       <c r="C294" s="3" t="inlineStr">
@@ -8403,19 +8403,19 @@
       </c>
       <c r="E294" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="4" t="inlineStr">
         <is>
-          <t>210939</t>
+          <t>210840</t>
         </is>
       </c>
       <c r="B295" s="4" t="inlineStr">
         <is>
-          <t>خليل جبر احمد على العبيى</t>
+          <t>يونس دينى اسماعيل</t>
         </is>
       </c>
       <c r="C295" s="4" t="inlineStr">
@@ -8430,19 +8430,19 @@
       </c>
       <c r="E295" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="3" t="inlineStr">
         <is>
-          <t>210941</t>
+          <t>210939</t>
         </is>
       </c>
       <c r="B296" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">مصطفى امين غانم  </t>
+          <t>خليل جبر احمد على العبيى</t>
         </is>
       </c>
       <c r="C296" s="3" t="inlineStr">
@@ -8457,19 +8457,19 @@
       </c>
       <c r="E296" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="4" t="inlineStr">
         <is>
-          <t>210947</t>
+          <t>210941</t>
         </is>
       </c>
       <c r="B297" s="4" t="inlineStr">
         <is>
-          <t>مريم بنت يعقوب بن يوسف الحمود</t>
+          <t xml:space="preserve">مصطفى امين غانم  </t>
         </is>
       </c>
       <c r="C297" s="4" t="inlineStr">
@@ -8484,19 +8484,19 @@
       </c>
       <c r="E297" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="3" t="inlineStr">
         <is>
-          <t>210965</t>
+          <t>210947</t>
         </is>
       </c>
       <c r="B298" s="3" t="inlineStr">
         <is>
-          <t>همام احمد خليل</t>
+          <t>مريم بنت يعقوب بن يوسف الحمود</t>
         </is>
       </c>
       <c r="C298" s="3" t="inlineStr">
@@ -8511,19 +8511,19 @@
       </c>
       <c r="E298" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="4" t="inlineStr">
         <is>
-          <t>210982</t>
+          <t>210965</t>
         </is>
       </c>
       <c r="B299" s="4" t="inlineStr">
         <is>
-          <t>عمر نصر الدين محمد خالد صب لبن</t>
+          <t>همام احمد خليل</t>
         </is>
       </c>
       <c r="C299" s="4" t="inlineStr">
@@ -8538,19 +8538,19 @@
       </c>
       <c r="E299" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="3" t="inlineStr">
         <is>
-          <t>210984</t>
+          <t>210982</t>
         </is>
       </c>
       <c r="B300" s="3" t="inlineStr">
         <is>
-          <t>وسيم رزق محمد سهمود</t>
+          <t>عمر نصر الدين محمد خالد صب لبن</t>
         </is>
       </c>
       <c r="C300" s="3" t="inlineStr">
@@ -8565,19 +8565,19 @@
       </c>
       <c r="E300" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="4" t="inlineStr">
         <is>
-          <t>210994</t>
+          <t>210984</t>
         </is>
       </c>
       <c r="B301" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">نور ماجد فايز ابو جامع </t>
+          <t>وسيم رزق محمد سهمود</t>
         </is>
       </c>
       <c r="C301" s="4" t="inlineStr">
@@ -8592,19 +8592,19 @@
       </c>
       <c r="E301" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="3" t="inlineStr">
         <is>
-          <t>211002</t>
+          <t>210994</t>
         </is>
       </c>
       <c r="B302" s="3" t="inlineStr">
         <is>
-          <t>منيه خالد الشيخ حاج محمود</t>
+          <t xml:space="preserve">نور ماجد فايز ابو جامع </t>
         </is>
       </c>
       <c r="C302" s="3" t="inlineStr">
@@ -8619,19 +8619,19 @@
       </c>
       <c r="E302" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="4" t="inlineStr">
         <is>
-          <t>211003</t>
+          <t>211002</t>
         </is>
       </c>
       <c r="B303" s="4" t="inlineStr">
         <is>
-          <t>محمد عادل محمد عبد الله العريفى</t>
+          <t>منيه خالد الشيخ حاج محمود</t>
         </is>
       </c>
       <c r="C303" s="4" t="inlineStr">
@@ -8646,19 +8646,19 @@
       </c>
       <c r="E303" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="3" t="inlineStr">
         <is>
-          <t>211005</t>
+          <t>211003</t>
         </is>
       </c>
       <c r="B304" s="3" t="inlineStr">
         <is>
-          <t>محمد باسم محمد على نويات</t>
+          <t>محمد عادل محمد عبد الله العريفى</t>
         </is>
       </c>
       <c r="C304" s="3" t="inlineStr">
@@ -8673,19 +8673,19 @@
       </c>
       <c r="E304" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="4" t="inlineStr">
         <is>
-          <t>211024</t>
+          <t>211005</t>
         </is>
       </c>
       <c r="B305" s="4" t="inlineStr">
         <is>
-          <t>جاسم محمد المحيمد الخلف</t>
+          <t>محمد باسم محمد على نويات</t>
         </is>
       </c>
       <c r="C305" s="4" t="inlineStr">
@@ -8700,19 +8700,19 @@
       </c>
       <c r="E305" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="3" t="inlineStr">
         <is>
-          <t>211025</t>
+          <t>211024</t>
         </is>
       </c>
       <c r="B306" s="3" t="inlineStr">
         <is>
-          <t>شموخ على محمد حمادى</t>
+          <t>جاسم محمد المحيمد الخلف</t>
         </is>
       </c>
       <c r="C306" s="3" t="inlineStr">
@@ -8727,19 +8727,19 @@
       </c>
       <c r="E306" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="4" t="inlineStr">
         <is>
-          <t>211029</t>
+          <t>211025</t>
         </is>
       </c>
       <c r="B307" s="4" t="inlineStr">
         <is>
-          <t>عبد الرحمن الضو النور على</t>
+          <t>شموخ على محمد حمادى</t>
         </is>
       </c>
       <c r="C307" s="4" t="inlineStr">
@@ -8754,19 +8754,19 @@
       </c>
       <c r="E307" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="3" t="inlineStr">
         <is>
-          <t>211044</t>
+          <t>211029</t>
         </is>
       </c>
       <c r="B308" s="3" t="inlineStr">
         <is>
-          <t>لجين فتحى عدلى محمد عبد الله</t>
+          <t>عبد الرحمن الضو النور على</t>
         </is>
       </c>
       <c r="C308" s="3" t="inlineStr">
@@ -8781,19 +8781,19 @@
       </c>
       <c r="E308" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="4" t="inlineStr">
         <is>
-          <t>211048</t>
+          <t>211044</t>
         </is>
       </c>
       <c r="B309" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">فادى نواف الحريرى </t>
+          <t>لجين فتحى عدلى محمد عبد الله</t>
         </is>
       </c>
       <c r="C309" s="4" t="inlineStr">
@@ -8808,19 +8808,19 @@
       </c>
       <c r="E309" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="3" t="inlineStr">
         <is>
-          <t>211056</t>
+          <t>211048</t>
         </is>
       </c>
       <c r="B310" s="3" t="inlineStr">
         <is>
-          <t>محمد وداد احمد وداد فرج</t>
+          <t xml:space="preserve">فادى نواف الحريرى </t>
         </is>
       </c>
       <c r="C310" s="3" t="inlineStr">
@@ -8835,19 +8835,19 @@
       </c>
       <c r="E310" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="4" t="inlineStr">
         <is>
-          <t>211060</t>
+          <t>211056</t>
         </is>
       </c>
       <c r="B311" s="4" t="inlineStr">
         <is>
-          <t>مروه فرحان الداموك</t>
+          <t>محمد وداد احمد وداد فرج</t>
         </is>
       </c>
       <c r="C311" s="4" t="inlineStr">
@@ -8862,19 +8862,19 @@
       </c>
       <c r="E311" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="3" t="inlineStr">
         <is>
-          <t>211063</t>
+          <t>211060</t>
         </is>
       </c>
       <c r="B312" s="3" t="inlineStr">
         <is>
-          <t>مايا مراد موسى عبد القادر</t>
+          <t>مروه فرحان الداموك</t>
         </is>
       </c>
       <c r="C312" s="3" t="inlineStr">
@@ -8889,19 +8889,19 @@
       </c>
       <c r="E312" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="4" t="inlineStr">
         <is>
-          <t>211069</t>
+          <t>211063</t>
         </is>
       </c>
       <c r="B313" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">احمد رياض محمد صافى </t>
+          <t>مايا مراد موسى عبد القادر</t>
         </is>
       </c>
       <c r="C313" s="4" t="inlineStr">
@@ -8916,19 +8916,19 @@
       </c>
       <c r="E313" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="3" t="inlineStr">
         <is>
-          <t>211073</t>
+          <t>211069</t>
         </is>
       </c>
       <c r="B314" s="3" t="inlineStr">
         <is>
-          <t>حنين ايمن فؤاد دغباج</t>
+          <t xml:space="preserve">احمد رياض محمد صافى </t>
         </is>
       </c>
       <c r="C314" s="3" t="inlineStr">
@@ -8943,19 +8943,19 @@
       </c>
       <c r="E314" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="4" t="inlineStr">
         <is>
-          <t>211934</t>
+          <t>211073</t>
         </is>
       </c>
       <c r="B315" s="4" t="inlineStr">
         <is>
-          <t>زيدون احمد محمود درادكه</t>
+          <t>حنين ايمن فؤاد دغباج</t>
         </is>
       </c>
       <c r="C315" s="4" t="inlineStr">
@@ -8970,19 +8970,19 @@
       </c>
       <c r="E315" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="3" t="inlineStr">
         <is>
-          <t>220467</t>
+          <t>211934</t>
         </is>
       </c>
       <c r="B316" s="3" t="inlineStr">
         <is>
-          <t>خليل صالح الحريري</t>
+          <t>زيدون احمد محمود درادكه</t>
         </is>
       </c>
       <c r="C316" s="3" t="inlineStr">
@@ -8997,19 +8997,19 @@
       </c>
       <c r="E316" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="4" t="inlineStr">
         <is>
-          <t>221082</t>
+          <t>220467</t>
         </is>
       </c>
       <c r="B317" s="4" t="inlineStr">
         <is>
-          <t>جنى ايمن احمد شديد</t>
+          <t>خليل صالح الحريري</t>
         </is>
       </c>
       <c r="C317" s="4" t="inlineStr">
@@ -9024,19 +9024,19 @@
       </c>
       <c r="E317" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="3" t="inlineStr">
         <is>
-          <t>221105</t>
+          <t>221082</t>
         </is>
       </c>
       <c r="B318" s="3" t="inlineStr">
         <is>
-          <t>ديفيد ادوار شكري برتلة رزق</t>
+          <t>جنى ايمن احمد شديد</t>
         </is>
       </c>
       <c r="C318" s="3" t="inlineStr">
@@ -9051,19 +9051,19 @@
       </c>
       <c r="E318" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="4" t="inlineStr">
         <is>
-          <t>223001</t>
+          <t>221105</t>
         </is>
       </c>
       <c r="B319" s="4" t="inlineStr">
         <is>
-          <t>زينه هانى فاروق محمد يوسف</t>
+          <t>ديفيد ادوار شكري برتلة رزق</t>
         </is>
       </c>
       <c r="C319" s="4" t="inlineStr">
@@ -9078,19 +9078,19 @@
       </c>
       <c r="E319" s="4" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="3" t="inlineStr">
         <is>
-          <t>223002</t>
+          <t>223001</t>
         </is>
       </c>
       <c r="B320" s="3" t="inlineStr">
         <is>
-          <t>يسرا ضياء الدين نادى محمود الحينى</t>
+          <t>زينه هانى فاروق محمد يوسف</t>
         </is>
       </c>
       <c r="C320" s="3" t="inlineStr">
@@ -9105,34 +9105,61 @@
       </c>
       <c r="E320" s="3" t="inlineStr">
         <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="4" t="inlineStr">
         <is>
+          <t>223002</t>
+        </is>
+      </c>
+      <c r="B321" s="4" t="inlineStr">
+        <is>
+          <t>يسرا ضياء الدين نادى محمود الحينى</t>
+        </is>
+      </c>
+      <c r="C321" s="4" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="D321" s="4" t="inlineStr">
+        <is>
+          <t>B1F2</t>
+        </is>
+      </c>
+      <c r="E321" s="4" t="inlineStr">
+        <is>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" s="3" t="inlineStr">
+        <is>
           <t>223007</t>
         </is>
       </c>
-      <c r="B321" s="4" t="inlineStr">
+      <c r="B322" s="3" t="inlineStr">
         <is>
           <t>خالد احمد محمد الكردى</t>
         </is>
       </c>
-      <c r="C321" s="4" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="D321" s="4" t="inlineStr">
+      <c r="C322" s="3" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="D322" s="3" t="inlineStr">
         <is>
           <t>B1F2</t>
         </is>
       </c>
-      <c r="E321" s="4" t="inlineStr">
-        <is>
-          <t>Y4_B2526_General_&amp;_Special_Surgery_1_B1_reference_data.xlsx</t>
+      <c r="E322" s="3" t="inlineStr">
+        <is>
+          <t>Y4_B2526_General_&amp;_Special_surgery_1_B1_reference_data_D23122025T104608.xlsx</t>
         </is>
       </c>
     </row>

</xml_diff>